<commit_message>
wallet transaction history been updated,wishlist updated
</commit_message>
<xml_diff>
--- a/public/files/data.xlsx
+++ b/public/files/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -466,9 +466,457 @@
         <v>Delivered</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v xml:space="preserve">Wed Feb 15 2023 </v>
+      </c>
+      <c r="B3" t="str">
+        <v>trideep kumar</v>
+      </c>
+      <c r="C3" t="str">
+        <v>trideep@gmail.com</v>
+      </c>
+      <c r="D3" t="str">
+        <v>9061117489</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Casio G-Shock Gold Dial Mens Watch-G1053</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Black and Gold</v>
+      </c>
+      <c r="H3">
+        <v>76030</v>
+      </c>
+      <c r="I3" t="str">
+        <v>RAZORPAY</v>
+      </c>
+      <c r="J3" t="str">
+        <v>Placed</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v xml:space="preserve">Fri Feb 17 2023 </v>
+      </c>
+      <c r="B4" t="str">
+        <v xml:space="preserve">Mazin </v>
+      </c>
+      <c r="C4" t="str">
+        <v>mazinshajahan4444@gmail.com</v>
+      </c>
+      <c r="D4" t="str">
+        <v>7510722928</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Casio G-Shock Gold Dial Mens Watch-G1053</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="str">
+        <v>Black and Gold</v>
+      </c>
+      <c r="H4">
+        <v>19045</v>
+      </c>
+      <c r="I4" t="str">
+        <v>COD</v>
+      </c>
+      <c r="J4" t="str">
+        <v>Delivered</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v xml:space="preserve">Sat Feb 18 2023 </v>
+      </c>
+      <c r="B5" t="str">
+        <v>Muhammed Musthafa</v>
+      </c>
+      <c r="C5" t="str">
+        <v>musthafa723262@gmail.com</v>
+      </c>
+      <c r="D5" t="str">
+        <v>9544535049</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Mens 45.9 mm Daniel Black Dial Zinc Alloy Watch - NCTH1710383</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="str">
+        <v>black</v>
+      </c>
+      <c r="H5">
+        <v>13300</v>
+      </c>
+      <c r="I5" t="str">
+        <v>Wallet</v>
+      </c>
+      <c r="J5" t="str">
+        <v>Placed</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v xml:space="preserve">Sat Feb 18 2023 </v>
+      </c>
+      <c r="B6" t="str">
+        <v>Muhammed Musthafa</v>
+      </c>
+      <c r="C6" t="str">
+        <v>musthafa723262@gmail.com</v>
+      </c>
+      <c r="D6" t="str">
+        <v>9544535049</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Mens 45.9 mm Daniel Black Dial Zinc Alloy Watch - NCTH1710383</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="str">
+        <v>black</v>
+      </c>
+      <c r="H6">
+        <v>13300</v>
+      </c>
+      <c r="I6" t="str">
+        <v>Wallet</v>
+      </c>
+      <c r="J6" t="str">
+        <v>Delivered</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">Sat Feb 18 2023 </v>
+      </c>
+      <c r="B7" t="str">
+        <v>Muhammed Musthafa</v>
+      </c>
+      <c r="C7" t="str">
+        <v>musthafa723262@gmail.com</v>
+      </c>
+      <c r="D7" t="str">
+        <v>9544535049</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Casio Edifice Black Dial Men's Watch -EX511</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="str">
+        <v>silver</v>
+      </c>
+      <c r="H7">
+        <v>30045</v>
+      </c>
+      <c r="I7" t="str">
+        <v>Wallet</v>
+      </c>
+      <c r="J7" t="str">
+        <v>Delivered</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve">Sat Feb 18 2023 </v>
+      </c>
+      <c r="B8" t="str">
+        <v>Muhammed Musthafa</v>
+      </c>
+      <c r="C8" t="str">
+        <v>musthafa723262@gmail.com</v>
+      </c>
+      <c r="D8" t="str">
+        <v>9544535049</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Mens 45.9 mm Daniel Black Dial Zinc Alloy Watch - NCTH1710383</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="str">
+        <v>black</v>
+      </c>
+      <c r="H8">
+        <v>13300</v>
+      </c>
+      <c r="I8" t="str">
+        <v>Wallet</v>
+      </c>
+      <c r="J8" t="str">
+        <v>Placed</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v xml:space="preserve">Sat Feb 18 2023 </v>
+      </c>
+      <c r="B9" t="str">
+        <v>Muhammed Musthafa</v>
+      </c>
+      <c r="C9" t="str">
+        <v>musthafa723262@gmail.com</v>
+      </c>
+      <c r="D9" t="str">
+        <v>9544535049</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Mens 45.9 mm Daniel Black Dial Zinc Alloy Watch - NCTH1710383</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="str">
+        <v>black</v>
+      </c>
+      <c r="H9">
+        <v>13300</v>
+      </c>
+      <c r="I9" t="str">
+        <v>Wallet</v>
+      </c>
+      <c r="J9" t="str">
+        <v>Placed</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v xml:space="preserve">Sat Feb 18 2023 </v>
+      </c>
+      <c r="B10" t="str">
+        <v>Muhammed Musthafa</v>
+      </c>
+      <c r="C10" t="str">
+        <v>musthafa723262@gmail.com</v>
+      </c>
+      <c r="D10" t="str">
+        <v>9544535049</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Mens 45.9 mm Daniel Black Dial Zinc Alloy Watch - NCTH1710383</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="str">
+        <v>black</v>
+      </c>
+      <c r="H10">
+        <v>20455</v>
+      </c>
+      <c r="I10" t="str">
+        <v>Wallet</v>
+      </c>
+      <c r="J10" t="str">
+        <v>Placed</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v xml:space="preserve">Sat Feb 18 2023 </v>
+      </c>
+      <c r="B11" t="str">
+        <v>Muhammed Musthafa</v>
+      </c>
+      <c r="C11" t="str">
+        <v>musthafa723262@gmail.com</v>
+      </c>
+      <c r="D11" t="str">
+        <v>9544535049</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Mens 45.9 mm Daniel Black Dial Zinc Alloy Watch - NCTH1710383</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="str">
+        <v>black</v>
+      </c>
+      <c r="H11">
+        <v>13300</v>
+      </c>
+      <c r="I11" t="str">
+        <v>Wallet</v>
+      </c>
+      <c r="J11" t="str">
+        <v>Placed</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v xml:space="preserve">Sat Feb 18 2023 </v>
+      </c>
+      <c r="B12" t="str">
+        <v>Muhammed Musthafa</v>
+      </c>
+      <c r="C12" t="str">
+        <v>musthafa723262@gmail.com</v>
+      </c>
+      <c r="D12" t="str">
+        <v>9544535049</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Mens 45.9 mm Daniel Black Dial Zinc Alloy Watch - NCTH1710383</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="str">
+        <v>black</v>
+      </c>
+      <c r="H12">
+        <v>11710</v>
+      </c>
+      <c r="I12" t="str">
+        <v>Wallet</v>
+      </c>
+      <c r="J12" t="str">
+        <v>Placed</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v xml:space="preserve">Sat Feb 18 2023 </v>
+      </c>
+      <c r="B13" t="str">
+        <v>Muhammed Musthafa</v>
+      </c>
+      <c r="C13" t="str">
+        <v>musthafa723262@gmail.com</v>
+      </c>
+      <c r="D13" t="str">
+        <v>9544535049</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Mens 45.9 mm Daniel Black Dial Zinc Alloy Watch - NCTH1710383</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="str">
+        <v>black</v>
+      </c>
+      <c r="H13">
+        <v>11710</v>
+      </c>
+      <c r="I13" t="str">
+        <v>Wallet</v>
+      </c>
+      <c r="J13" t="str">
+        <v>Placed</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v xml:space="preserve">Sat Feb 18 2023 </v>
+      </c>
+      <c r="B14" t="str">
+        <v>Musthafa</v>
+      </c>
+      <c r="C14" t="str">
+        <v>musthafa916@gmail.com</v>
+      </c>
+      <c r="D14" t="str">
+        <v>9047792111</v>
+      </c>
+      <c r="E14" t="str">
+        <v>DAY-DATE 40</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14" t="str">
+        <v xml:space="preserve"> yellow gold and diamonds</v>
+      </c>
+      <c r="H14">
+        <v>3136350</v>
+      </c>
+      <c r="I14" t="str">
+        <v>COD</v>
+      </c>
+      <c r="J14" t="str">
+        <v>Delivered</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v xml:space="preserve">Mon Feb 20 2023 </v>
+      </c>
+      <c r="B15" t="str">
+        <v>neeraj</v>
+      </c>
+      <c r="C15" t="str">
+        <v>ifoxscand@gmail.com</v>
+      </c>
+      <c r="D15" t="str">
+        <v>9074165714</v>
+      </c>
+      <c r="E15" t="str">
+        <v>Casio G-Shock Gold Dial Mens Watch-G1053</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="str">
+        <v>Black and Gold</v>
+      </c>
+      <c r="H15">
+        <v>19045</v>
+      </c>
+      <c r="I15" t="str">
+        <v>COD</v>
+      </c>
+      <c r="J15" t="str">
+        <v>Delivered</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v xml:space="preserve">Mon Feb 20 2023 </v>
+      </c>
+      <c r="B16" t="str">
+        <v>neeraj</v>
+      </c>
+      <c r="C16" t="str">
+        <v>ifoxscand@gmail.com</v>
+      </c>
+      <c r="D16" t="str">
+        <v>9074165714</v>
+      </c>
+      <c r="E16" t="str">
+        <v>Mens 45.9 mm Daniel Black Dial Zinc Alloy Watch - NCTH1710383</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="str">
+        <v>black</v>
+      </c>
+      <c r="H16">
+        <v>11710</v>
+      </c>
+      <c r="I16" t="str">
+        <v>RAZORPAY</v>
+      </c>
+      <c r="J16" t="str">
+        <v>Placed</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J16"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>